<commit_message>
Fixed some markdown links.
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\03-backend\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\public\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578AAF1A-DF9A-49DB-957F-C2A0229C3DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223E2F3F-CB24-4880-A204-10627F4DD6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Majority of the backend's documentation.</t>
   </si>
   <si>
-    <t>[/conf](/conf)</t>
-  </si>
-  <si>
     <t>[/docs](/docs)</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>Contains exports of Postman LUX-related requests and environment template.</t>
+  </si>
+  <si>
+    <t>[/config](/config)</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -614,16 +616,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -634,10 +636,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
@@ -645,217 +647,217 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>29</v>
-      </c>
-      <c r="H8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
         <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
         <v>13</v>
-      </c>
-      <c r="H21" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
         <v>51</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" t="s">
         <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
         <v>19</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>20</v>
-      </c>
-      <c r="H26" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -881,66 +883,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some markdown links. (#187)
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\03-backend\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\public\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578AAF1A-DF9A-49DB-957F-C2A0229C3DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223E2F3F-CB24-4880-A204-10627F4DD6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Majority of the backend's documentation.</t>
   </si>
   <si>
-    <t>[/conf](/conf)</t>
-  </si>
-  <si>
     <t>[/docs](/docs)</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>Contains exports of Postman LUX-related requests and environment template.</t>
+  </si>
+  <si>
+    <t>[/config](/config)</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -614,16 +616,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -634,10 +636,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
@@ -645,217 +647,217 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>29</v>
-      </c>
-      <c r="H8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
         <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
         <v>13</v>
-      </c>
-      <c r="H21" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
         <v>51</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" t="s">
         <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
         <v>19</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>20</v>
-      </c>
-      <c r="H26" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -881,66 +883,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#192: extracted the query plan viewer and bumped up the remaining modules directly within the ml-modules directory,
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\public\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223E2F3F-CB24-4880-A204-10627F4DD6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D613D2B0-3896-4DD7-8FDE-2754DC1C6E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>Path</t>
   </si>
@@ -121,42 +121,6 @@
     <t>[/base](/src/main/ml-config/base)</t>
   </si>
   <si>
-    <t>All of the project's module directories.  Selected ones may vary by environment.</t>
-  </si>
-  <si>
-    <t>[/base](/src/main/ml-modules/base)</t>
-  </si>
-  <si>
-    <t>[/options](/src/main/ml-modules/base/options)</t>
-  </si>
-  <si>
-    <t>[/root](/src/main/ml-modules/base/root)</t>
-  </si>
-  <si>
-    <t>[/ds](/src/main/ml-modules/base/root/ds)</t>
-  </si>
-  <si>
-    <t>[/lib](/src/main/ml-modules/base/root/lib)</t>
-  </si>
-  <si>
-    <t>[/utils](/src/main/ml-modules/base/root/utils)</t>
-  </si>
-  <si>
-    <t>The base modules applicable to all environments.</t>
-  </si>
-  <si>
-    <t>[/query-plan-viewer](/src/main/ml-modules/query-plan-viewer)</t>
-  </si>
-  <si>
-    <t>The modules needed by the Query Plan Viewer.</t>
-  </si>
-  <si>
-    <t>[/query-plan-viewer](/src/main/ml-config/query-plan-viewer)</t>
-  </si>
-  <si>
-    <t>[/query-plan-viewer-secured](/src/main/ml-config/query-plan-viewer-secured)</t>
-  </si>
-  <si>
     <t>[/base-unsecured](/src/main/ml-config/base-unsecured)</t>
   </si>
   <si>
@@ -169,27 +133,18 @@
     <t>The base configuration directory applicable to all environments.  It includes the group configuration, main content database, roles, and application servers.</t>
   </si>
   <si>
-    <t>A developer tool that helps one visualize an otherwise dense XML-formatted query plan.  Query Console also includes one.  However, at least through MarkLogic version 10.0-9, the one integrated within Query Console is only usable when the query type is SPARQL or SQL.  We need it for JavaScript.  The configuration is limited to an application server whose root directory is `/query-plan-viewer`.  The source code is copied from https://github.com/jpcs/queryplan-viewer into [/src/main/ml-modules/query-plan-viewer/root/query-plan-viewer](/src/main/ml-modules/query-plan-viewer/root/query-plan-viewer).  Locally, the URL is http://localhost:8006/default.xqy.</t>
-  </si>
-  <si>
     <t>The build script.</t>
   </si>
   <si>
     <t>The heart of LUX's backend implementation, where developers get to spend most of their time when they're lucky :)</t>
   </si>
   <si>
-    <t>[/runDuringDeployment](/src/main/ml-modules/base/root/runDuringDeployment)</t>
-  </si>
-  <si>
     <t>[LUX Gradle Tasks](/docs/lux-backend-build-tool-and-tasks.md#lux-gradle-tasks), [Data Constants](/docs/lux-backend-data-constants.md)</t>
   </si>
   <si>
     <t>HTTPS settings that stack on top of the base configuration.</t>
   </si>
   <si>
-    <t>HTTPS settings for the query plan viewer's app server.</t>
-  </si>
-  <si>
     <t>How</t>
   </si>
   <si>
@@ -238,12 +193,6 @@
     <t>http[s]://[hostname]:8002/history.  As the top-level charts can be the sum of all nodes, click into each category to access node-specific details and additional charts.  Available information includes IO wait time, swap, HTTP request counts, XQDP request counts, XQDP response times, and more.</t>
   </si>
   <si>
-    <t>[/config](/src/main/ml-modules/base/root/config)</t>
-  </si>
-  <si>
-    <t>[/data](/src/main/ml-modules/base/root/data)</t>
-  </si>
-  <si>
     <t>Configuration for search, facets, and more.  Includes placeholder files that are replaced during deployment.</t>
   </si>
   <si>
@@ -260,6 +209,33 @@
   </si>
   <si>
     <t>[/config](/config)</t>
+  </si>
+  <si>
+    <t>[/root](/src/main/ml-modules/root)</t>
+  </si>
+  <si>
+    <t>[/options](/src/main/ml-modules/options)</t>
+  </si>
+  <si>
+    <t>The modules applicable to all environments.</t>
+  </si>
+  <si>
+    <t>[/config](/src/main/ml-modules/root/config)</t>
+  </si>
+  <si>
+    <t>[/data](/src/main/ml-modules/root/data)</t>
+  </si>
+  <si>
+    <t>[/ds](/src/main/ml-modules/root/ds)</t>
+  </si>
+  <si>
+    <t>[/lib](/src/main/ml-modules/root/lib)</t>
+  </si>
+  <si>
+    <t>[/runDuringDeployment](/src/main/ml-modules/root/runDuringDeployment)</t>
+  </si>
+  <si>
+    <t>[/utils](/src/main/ml-modules/root/utils)</t>
   </si>
 </sst>
 </file>
@@ -597,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -636,7 +612,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -661,7 +637,7 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
@@ -685,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -704,159 +680,127 @@
         <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D12" t="s">
-        <v>41</v>
+      <c r="C12" t="s">
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D13" t="s">
-        <v>42</v>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
+      <c r="D15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" t="s">
-        <v>38</v>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" t="s">
-        <v>10</v>
+        <v>65</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E18" t="s">
-        <v>34</v>
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
       <c r="F19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
       <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
         <v>35</v>
       </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="F23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" t="s">
-        <v>74</v>
-      </c>
       <c r="H23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="F24" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" t="s">
         <v>14</v>
       </c>
     </row>
@@ -883,66 +827,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#290: removed facetProductMaximum property, removed associated documentation and code, and updated repo documentation starting from spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\public\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D613D2B0-3896-4DD7-8FDE-2754DC1C6E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F651BCF4-9295-473C-97E3-3C8EAE3941FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>The heart of LUX's backend implementation, where developers get to spend most of their time when they're lucky :)</t>
   </si>
   <si>
-    <t>[LUX Gradle Tasks](/docs/lux-backend-build-tool-and-tasks.md#lux-gradle-tasks), [Data Constants](/docs/lux-backend-data-constants.md)</t>
-  </si>
-  <si>
     <t>HTTPS settings that stack on top of the base configuration.</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>Includes the words to exclude from search criteria.</t>
   </si>
   <si>
-    <t>Includes scripts to deploy then execute during deployment, directly supporting generators for the data constants, remaining search terms, related lists, and advanced search configuration.</t>
-  </si>
-  <si>
     <t>All of the project's runtime code, most of its MarkLogic configuration, and some data all within ML Gradle's conventions.</t>
   </si>
   <si>
@@ -236,6 +230,12 @@
   </si>
   <si>
     <t>[/utils](/src/main/ml-modules/root/utils)</t>
+  </si>
+  <si>
+    <t>Includes scripts to deploy then execute during deployment, directly supporting generators for the remaining search terms, related lists, and advanced search configuration.</t>
+  </si>
+  <si>
+    <t>[LUX Gradle Tasks](/docs/lux-backend-build-tool-and-tasks.md#lux-gradle-tasks)</t>
   </si>
 </sst>
 </file>
@@ -573,21 +573,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="9.23046875" customWidth="1"/>
+    <col min="5" max="5" width="65.53515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57" customWidth="1"/>
     <col min="7" max="7" width="85.15234375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="95.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,150 +603,150 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
       <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
       <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>21</v>
       </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
       <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>27</v>
       </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="G10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" t="s">
+      <c r="F12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E18" t="s">
         <v>64</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="E18" t="s">
-        <v>66</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -755,52 +755,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" t="s">
         <v>68</v>
       </c>
-      <c r="F20" t="s">
-        <v>57</v>
-      </c>
       <c r="G20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
         <v>18</v>
       </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
       <c r="G22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>16</v>
       </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
       <c r="G23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -827,66 +827,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation updates: fixed links, typos, versions, etc.
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\public\lux-marklogic\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F651BCF4-9295-473C-97E3-3C8EAE3941FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BA395C-2FD7-4A89-9BAA-1A3D49D17150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>Path</t>
   </si>
@@ -85,12 +85,6 @@
     <t>[/templates](/src/main/templates)</t>
   </si>
   <si>
-    <t>JavaScript template files used by [/build.gradle](/build.gradle)</t>
-  </si>
-  <si>
-    <t>[JavaScript Template Files](/docs/lux-backend-build-tool-and-tasks.md#javascript-template-files)</t>
-  </si>
-  <si>
     <t>[/postman](/postman)</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>All of the project's ML Gradle configuration directories.  Selected ones may vary by environment.</t>
   </si>
   <si>
-    <t>[Gradle Properties](/docs/lux-backend-deployment.md#gradle-properties)</t>
-  </si>
-  <si>
     <t>[/base](/src/main/ml-config/base)</t>
   </si>
   <si>
@@ -127,12 +118,6 @@
     <t>[/base-secured](/src/main/ml-config/base-secured)</t>
   </si>
   <si>
-    <t>Defines a local, non-admin user to perform most of deployments with.</t>
-  </si>
-  <si>
-    <t>The base configuration directory applicable to all environments.  It includes the group configuration, main content database, roles, and application servers.</t>
-  </si>
-  <si>
     <t>The build script.</t>
   </si>
   <si>
@@ -236,6 +221,18 @@
   </si>
   <si>
     <t>[LUX Gradle Tasks](/docs/lux-backend-build-tool-and-tasks.md#lux-gradle-tasks)</t>
+  </si>
+  <si>
+    <t>The base configuration directory applicable to all tenants.  It includes the group configuration, main content database, roles, and application servers.</t>
+  </si>
+  <si>
+    <t>Intended for local developer environments.  Defines a local, non-admin user to perform most of deployments with plus some endpoint consumers.</t>
+  </si>
+  <si>
+    <t>[Tenant Configuration](/docs/lux-backend-deployment.md#tenant-configuration)</t>
+  </si>
+  <si>
+    <t>Reserved for JavaScript template files used by [/build.gradle](/build.gradle).</t>
   </si>
 </sst>
 </file>
@@ -612,10 +609,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -634,13 +631,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -648,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -661,50 +658,50 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
         <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -712,12 +709,12 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -725,28 +722,28 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -757,26 +754,26 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -787,10 +784,7 @@
         <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
@@ -798,7 +792,7 @@
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -827,66 +821,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation updates: fixed links, typos, versions, etc. (#410)
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\public\lux-marklogic\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F651BCF4-9295-473C-97E3-3C8EAE3941FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BA395C-2FD7-4A89-9BAA-1A3D49D17150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>Path</t>
   </si>
@@ -85,12 +85,6 @@
     <t>[/templates](/src/main/templates)</t>
   </si>
   <si>
-    <t>JavaScript template files used by [/build.gradle](/build.gradle)</t>
-  </si>
-  <si>
-    <t>[JavaScript Template Files](/docs/lux-backend-build-tool-and-tasks.md#javascript-template-files)</t>
-  </si>
-  <si>
     <t>[/postman](/postman)</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>All of the project's ML Gradle configuration directories.  Selected ones may vary by environment.</t>
   </si>
   <si>
-    <t>[Gradle Properties](/docs/lux-backend-deployment.md#gradle-properties)</t>
-  </si>
-  <si>
     <t>[/base](/src/main/ml-config/base)</t>
   </si>
   <si>
@@ -127,12 +118,6 @@
     <t>[/base-secured](/src/main/ml-config/base-secured)</t>
   </si>
   <si>
-    <t>Defines a local, non-admin user to perform most of deployments with.</t>
-  </si>
-  <si>
-    <t>The base configuration directory applicable to all environments.  It includes the group configuration, main content database, roles, and application servers.</t>
-  </si>
-  <si>
     <t>The build script.</t>
   </si>
   <si>
@@ -236,6 +221,18 @@
   </si>
   <si>
     <t>[LUX Gradle Tasks](/docs/lux-backend-build-tool-and-tasks.md#lux-gradle-tasks)</t>
+  </si>
+  <si>
+    <t>The base configuration directory applicable to all tenants.  It includes the group configuration, main content database, roles, and application servers.</t>
+  </si>
+  <si>
+    <t>Intended for local developer environments.  Defines a local, non-admin user to perform most of deployments with plus some endpoint consumers.</t>
+  </si>
+  <si>
+    <t>[Tenant Configuration](/docs/lux-backend-deployment.md#tenant-configuration)</t>
+  </si>
+  <si>
+    <t>Reserved for JavaScript template files used by [/build.gradle](/build.gradle).</t>
   </si>
 </sst>
 </file>
@@ -612,10 +609,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -634,13 +631,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -648,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -661,50 +658,50 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
         <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -712,12 +709,12 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -725,28 +722,28 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -757,26 +754,26 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -787,10 +784,7 @@
         <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
@@ -798,7 +792,7 @@
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -827,66 +821,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="131.15" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added /src/test to repo inventory
</commit_message>
<xml_diff>
--- a/docs/lux-markdown-tables.xlsx
+++ b/docs/lux-markdown-tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\lux-marklogic\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BA395C-2FD7-4A89-9BAA-1A3D49D17150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA00D6D-A59B-4379-A824-68D03D0BAA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t>Path</t>
   </si>
@@ -233,6 +233,27 @@
   </si>
   <si>
     <t>Reserved for JavaScript template files used by [/build.gradle](/build.gradle).</t>
+  </si>
+  <si>
+    <t>[/test](/src/test)</t>
+  </si>
+  <si>
+    <t>[/ml-config](/src/test/ml-config)</t>
+  </si>
+  <si>
+    <t>Configuration required to execute unit tests, including roles and users.</t>
+  </si>
+  <si>
+    <t>Conditionally deployed by the `restrictUnitTestingDeployment` Gradle task.</t>
+  </si>
+  <si>
+    <t>[/ml-modules](/src/test/ml-modules)</t>
+  </si>
+  <si>
+    <t>All test suites, which can also include test data.</t>
+  </si>
+  <si>
+    <t>[MarkLogic Unit Test user guide](https://marklogic-community.github.io/marklogic-unit-test/)</t>
   </si>
 </sst>
 </file>
@@ -570,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G23"/>
+      <selection sqref="A1:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -788,13 +809,40 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G26" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>